<commit_message>
8 paskaita - Grid
</commit_message>
<xml_diff>
--- a/HTML ir CSS/8 paskaita - 12.29 - Grid/grid.xlsx
+++ b/HTML ir CSS/8 paskaita - 12.29 - Grid/grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Darbas\CodeAcademy\2023+\FEU12\praktika\HTML ir CSS\8 paskaita - 12.29 - Grid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C5EDE3-39BD-459E-BE1F-9C1E689F5A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700F9B8F-7DF9-4248-9AC3-7AFF8E209161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -51,14 +51,130 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -340,208 +456,636 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="G6:L28"/>
+  <dimension ref="G6:X79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="T61" sqref="T61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="3.28515625" customWidth="1"/>
     <col min="10" max="10" width="26.42578125" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="22"/>
+    <col min="24" max="24" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
     </row>
     <row r="7" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
     </row>
     <row r="8" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="7:12" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
     </row>
     <row r="10" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
     </row>
     <row r="11" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
     </row>
     <row r="12" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
     </row>
     <row r="13" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
     </row>
     <row r="14" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
     </row>
     <row r="15" spans="7:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
     </row>
     <row r="16" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
     </row>
     <row r="17" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
     </row>
     <row r="18" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
     </row>
     <row r="19" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
     </row>
     <row r="20" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
     </row>
     <row r="21" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
     </row>
     <row r="22" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
     </row>
     <row r="23" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
     </row>
     <row r="24" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
     </row>
     <row r="25" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
     </row>
     <row r="26" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
     </row>
     <row r="27" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
     </row>
     <row r="28" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="47" spans="15:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P47" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>2</v>
+      </c>
+      <c r="R47" s="1">
+        <v>3</v>
+      </c>
+      <c r="S47" s="1">
+        <v>4</v>
+      </c>
+      <c r="T47" s="1">
+        <v>5</v>
+      </c>
+      <c r="U47" s="1">
+        <v>6</v>
+      </c>
+      <c r="V47" s="1">
+        <v>7</v>
+      </c>
+      <c r="W47" s="1">
+        <v>8</v>
+      </c>
+      <c r="X47" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="15:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O48" s="22">
+        <v>1</v>
+      </c>
+      <c r="P48" s="9"/>
+      <c r="Q48" s="10"/>
+      <c r="R48" s="10">
+        <v>1</v>
+      </c>
+      <c r="S48" s="10">
+        <v>2</v>
+      </c>
+      <c r="T48" s="10">
+        <v>3</v>
+      </c>
+      <c r="U48" s="10">
+        <v>4</v>
+      </c>
+      <c r="V48" s="10">
+        <v>5</v>
+      </c>
+      <c r="W48" s="10">
+        <v>6</v>
+      </c>
+      <c r="X48" s="11"/>
+    </row>
+    <row r="49" spans="15:24" x14ac:dyDescent="0.25">
+      <c r="O49" s="22">
+        <v>2</v>
+      </c>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="23">
+        <v>1</v>
+      </c>
+      <c r="R49" s="13"/>
+      <c r="S49" s="14"/>
+      <c r="T49" s="14"/>
+      <c r="U49" s="14"/>
+      <c r="V49" s="14"/>
+      <c r="W49" s="15"/>
+      <c r="X49" s="5"/>
+    </row>
+    <row r="50" spans="15:24" x14ac:dyDescent="0.25">
+      <c r="O50" s="22">
+        <v>3</v>
+      </c>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="23">
+        <v>2</v>
+      </c>
+      <c r="R50" s="16"/>
+      <c r="S50" s="12"/>
+      <c r="T50" s="12"/>
+      <c r="U50" s="17"/>
+      <c r="V50" s="12"/>
+      <c r="W50" s="18"/>
+      <c r="X50" s="5"/>
+    </row>
+    <row r="51" spans="15:24" x14ac:dyDescent="0.25">
+      <c r="O51" s="22">
+        <v>4</v>
+      </c>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="23">
+        <v>3</v>
+      </c>
+      <c r="R51" s="16"/>
+      <c r="S51" s="12"/>
+      <c r="T51" s="12"/>
+      <c r="U51" s="17"/>
+      <c r="V51" s="12"/>
+      <c r="W51" s="18"/>
+      <c r="X51" s="5"/>
+    </row>
+    <row r="52" spans="15:24" x14ac:dyDescent="0.25">
+      <c r="O52" s="22">
+        <v>5</v>
+      </c>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="23">
+        <v>4</v>
+      </c>
+      <c r="R52" s="16"/>
+      <c r="S52" s="12"/>
+      <c r="T52" s="12"/>
+      <c r="U52" s="17"/>
+      <c r="V52" s="12"/>
+      <c r="W52" s="18"/>
+      <c r="X52" s="5"/>
+    </row>
+    <row r="53" spans="15:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O53" s="22">
+        <v>6</v>
+      </c>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="23">
+        <v>5</v>
+      </c>
+      <c r="R53" s="19"/>
+      <c r="S53" s="20"/>
+      <c r="T53" s="20"/>
+      <c r="U53" s="20"/>
+      <c r="V53" s="20"/>
+      <c r="W53" s="21"/>
+      <c r="X53" s="5"/>
+    </row>
+    <row r="54" spans="15:24" x14ac:dyDescent="0.25">
+      <c r="O54" s="22">
+        <v>7</v>
+      </c>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="4"/>
+      <c r="U54" s="4"/>
+      <c r="V54" s="4"/>
+      <c r="W54" s="4"/>
+      <c r="X54" s="5"/>
+    </row>
+    <row r="55" spans="15:24" x14ac:dyDescent="0.25">
+      <c r="P55" s="3"/>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
+      <c r="S55" s="4"/>
+      <c r="T55" s="4"/>
+      <c r="U55" s="4"/>
+      <c r="V55" s="4"/>
+      <c r="W55" s="4"/>
+      <c r="X55" s="5"/>
+    </row>
+    <row r="56" spans="15:24" x14ac:dyDescent="0.25">
+      <c r="P56" s="3"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4"/>
+      <c r="T56" s="4"/>
+      <c r="U56" s="4"/>
+      <c r="V56" s="4"/>
+      <c r="W56" s="4"/>
+      <c r="X56" s="5"/>
+    </row>
+    <row r="57" spans="15:24" x14ac:dyDescent="0.25">
+      <c r="P57" s="3"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+      <c r="U57" s="4"/>
+      <c r="V57" s="4"/>
+      <c r="W57" s="4"/>
+      <c r="X57" s="5"/>
+    </row>
+    <row r="58" spans="15:24" x14ac:dyDescent="0.25">
+      <c r="P58" s="3"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
+      <c r="S58" s="4"/>
+      <c r="T58" s="4"/>
+      <c r="U58" s="4"/>
+      <c r="V58" s="4"/>
+      <c r="W58" s="4"/>
+      <c r="X58" s="5"/>
+    </row>
+    <row r="59" spans="15:24" x14ac:dyDescent="0.25">
+      <c r="P59" s="3"/>
+      <c r="Q59" s="4"/>
+      <c r="R59" s="4"/>
+      <c r="S59" s="4"/>
+      <c r="T59" s="4"/>
+      <c r="U59" s="4"/>
+      <c r="V59" s="4"/>
+      <c r="W59" s="4"/>
+      <c r="X59" s="5"/>
+    </row>
+    <row r="60" spans="15:24" x14ac:dyDescent="0.25">
+      <c r="P60" s="3"/>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="4"/>
+      <c r="S60" s="4"/>
+      <c r="T60" s="4"/>
+      <c r="U60" s="4"/>
+      <c r="V60" s="4"/>
+      <c r="W60" s="4"/>
+      <c r="X60" s="5"/>
+    </row>
+    <row r="61" spans="15:24" x14ac:dyDescent="0.25">
+      <c r="P61" s="3"/>
+      <c r="Q61" s="4"/>
+      <c r="R61" s="4"/>
+      <c r="S61" s="4"/>
+      <c r="T61" s="4"/>
+      <c r="U61" s="4"/>
+      <c r="V61" s="4"/>
+      <c r="W61" s="4"/>
+      <c r="X61" s="5"/>
+    </row>
+    <row r="62" spans="15:24" x14ac:dyDescent="0.25">
+      <c r="P62" s="3"/>
+      <c r="Q62" s="4"/>
+      <c r="R62" s="4"/>
+      <c r="S62" s="4"/>
+      <c r="T62" s="4"/>
+      <c r="U62" s="4"/>
+      <c r="V62" s="4"/>
+      <c r="W62" s="4"/>
+      <c r="X62" s="5"/>
+    </row>
+    <row r="63" spans="15:24" x14ac:dyDescent="0.25">
+      <c r="P63" s="3"/>
+      <c r="Q63" s="4"/>
+      <c r="R63" s="4"/>
+      <c r="S63" s="4"/>
+      <c r="T63" s="4"/>
+      <c r="U63" s="4"/>
+      <c r="V63" s="4"/>
+      <c r="W63" s="4"/>
+      <c r="X63" s="5"/>
+    </row>
+    <row r="64" spans="15:24" x14ac:dyDescent="0.25">
+      <c r="P64" s="3"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="4"/>
+      <c r="S64" s="4"/>
+      <c r="T64" s="4"/>
+      <c r="U64" s="4"/>
+      <c r="V64" s="4"/>
+      <c r="W64" s="4"/>
+      <c r="X64" s="5"/>
+    </row>
+    <row r="65" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P65" s="3"/>
+      <c r="Q65" s="4"/>
+      <c r="R65" s="4"/>
+      <c r="S65" s="4"/>
+      <c r="T65" s="4"/>
+      <c r="U65" s="4"/>
+      <c r="V65" s="4"/>
+      <c r="W65" s="4"/>
+      <c r="X65" s="5"/>
+    </row>
+    <row r="66" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P66" s="3"/>
+      <c r="Q66" s="4"/>
+      <c r="R66" s="4"/>
+      <c r="S66" s="4"/>
+      <c r="T66" s="4"/>
+      <c r="U66" s="4"/>
+      <c r="V66" s="4"/>
+      <c r="W66" s="4"/>
+      <c r="X66" s="5"/>
+    </row>
+    <row r="67" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P67" s="3"/>
+      <c r="Q67" s="4"/>
+      <c r="R67" s="4"/>
+      <c r="S67" s="4"/>
+      <c r="T67" s="4"/>
+      <c r="U67" s="4"/>
+      <c r="V67" s="4"/>
+      <c r="W67" s="4"/>
+      <c r="X67" s="5"/>
+    </row>
+    <row r="68" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P68" s="3"/>
+      <c r="Q68" s="4"/>
+      <c r="R68" s="4"/>
+      <c r="S68" s="4"/>
+      <c r="T68" s="4"/>
+      <c r="U68" s="4"/>
+      <c r="V68" s="4"/>
+      <c r="W68" s="4"/>
+      <c r="X68" s="5"/>
+    </row>
+    <row r="69" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P69" s="3"/>
+      <c r="Q69" s="4"/>
+      <c r="R69" s="4"/>
+      <c r="S69" s="4"/>
+      <c r="T69" s="4"/>
+      <c r="U69" s="4"/>
+      <c r="V69" s="4"/>
+      <c r="W69" s="4"/>
+      <c r="X69" s="5"/>
+    </row>
+    <row r="70" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P70" s="3"/>
+      <c r="Q70" s="4"/>
+      <c r="R70" s="4"/>
+      <c r="S70" s="4"/>
+      <c r="T70" s="4"/>
+      <c r="U70" s="4"/>
+      <c r="V70" s="4"/>
+      <c r="W70" s="4"/>
+      <c r="X70" s="5"/>
+    </row>
+    <row r="71" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P71" s="3"/>
+      <c r="Q71" s="4"/>
+      <c r="R71" s="4"/>
+      <c r="S71" s="4"/>
+      <c r="T71" s="4"/>
+      <c r="U71" s="4"/>
+      <c r="V71" s="4"/>
+      <c r="W71" s="4"/>
+      <c r="X71" s="5"/>
+    </row>
+    <row r="72" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P72" s="3"/>
+      <c r="Q72" s="4"/>
+      <c r="R72" s="4"/>
+      <c r="S72" s="4"/>
+      <c r="T72" s="4"/>
+      <c r="U72" s="4"/>
+      <c r="V72" s="4"/>
+      <c r="W72" s="4"/>
+      <c r="X72" s="5"/>
+    </row>
+    <row r="73" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P73" s="3"/>
+      <c r="Q73" s="4"/>
+      <c r="R73" s="4"/>
+      <c r="S73" s="4"/>
+      <c r="T73" s="4"/>
+      <c r="U73" s="4"/>
+      <c r="V73" s="4"/>
+      <c r="W73" s="4"/>
+      <c r="X73" s="5"/>
+    </row>
+    <row r="74" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P74" s="3"/>
+      <c r="Q74" s="4"/>
+      <c r="R74" s="4"/>
+      <c r="S74" s="4"/>
+      <c r="T74" s="4"/>
+      <c r="U74" s="4"/>
+      <c r="V74" s="4"/>
+      <c r="W74" s="4"/>
+      <c r="X74" s="5"/>
+    </row>
+    <row r="75" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P75" s="3"/>
+      <c r="Q75" s="4"/>
+      <c r="R75" s="4"/>
+      <c r="S75" s="4"/>
+      <c r="T75" s="4"/>
+      <c r="U75" s="4"/>
+      <c r="V75" s="4"/>
+      <c r="W75" s="4"/>
+      <c r="X75" s="5"/>
+    </row>
+    <row r="76" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P76" s="3"/>
+      <c r="Q76" s="4"/>
+      <c r="R76" s="4"/>
+      <c r="S76" s="4"/>
+      <c r="T76" s="4"/>
+      <c r="U76" s="4"/>
+      <c r="V76" s="4"/>
+      <c r="W76" s="4"/>
+      <c r="X76" s="5"/>
+    </row>
+    <row r="77" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P77" s="3"/>
+      <c r="Q77" s="4"/>
+      <c r="R77" s="4"/>
+      <c r="S77" s="4"/>
+      <c r="T77" s="4"/>
+      <c r="U77" s="4"/>
+      <c r="V77" s="4"/>
+      <c r="W77" s="4"/>
+      <c r="X77" s="5"/>
+    </row>
+    <row r="78" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P78" s="3"/>
+      <c r="Q78" s="4"/>
+      <c r="R78" s="4"/>
+      <c r="S78" s="4"/>
+      <c r="T78" s="4"/>
+      <c r="U78" s="4"/>
+      <c r="V78" s="4"/>
+      <c r="W78" s="4"/>
+      <c r="X78" s="5"/>
+    </row>
+    <row r="79" spans="16:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P79" s="6"/>
+      <c r="Q79" s="7"/>
+      <c r="R79" s="7"/>
+      <c r="S79" s="7"/>
+      <c r="T79" s="7"/>
+      <c r="U79" s="7"/>
+      <c r="V79" s="7"/>
+      <c r="W79" s="7"/>
+      <c r="X79" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="G6:J10"/>
     <mergeCell ref="K6:L10"/>
     <mergeCell ref="G11:L13"/>
     <mergeCell ref="G14:L28"/>
+    <mergeCell ref="S50:T52"/>
+    <mergeCell ref="V50:V52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>